<commit_message>
mejora en los mensages de respuesta
</commit_message>
<xml_diff>
--- a/facundo.xlsx
+++ b/facundo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\comedores_unr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8470E4-FC90-4972-8DA5-52D7E7CDC3AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2610E022-18BD-403E-AF34-AA320D922A6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{5C91FBF1-797B-4D74-8CDC-7038822E3838}"/>
   </bookViews>
@@ -505,7 +505,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,7 +575,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C6" s="5">
         <v>45806</v>

</xml_diff>

<commit_message>
se comienza a incorporar la funcionalidad del mes
</commit_message>
<xml_diff>
--- a/facundo.xlsx
+++ b/facundo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\comedores_unr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2610E022-18BD-403E-AF34-AA320D922A6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14033E9-7160-4214-B092-57F11C89C1B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{5C91FBF1-797B-4D74-8CDC-7038822E3838}"/>
   </bookViews>
@@ -46,9 +46,6 @@
     <t>menu</t>
   </si>
   <si>
-    <t>dia_del_mes</t>
-  </si>
-  <si>
     <t>siberia</t>
   </si>
   <si>
@@ -119,6 +116,9 @@
   </si>
   <si>
     <t>cen_no_lleva</t>
+  </si>
+  <si>
+    <t>fecha</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,15 +523,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="5">
         <v>45803</v>
@@ -539,10 +539,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5">
         <v>45803</v>
@@ -550,10 +550,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="5">
         <v>45804</v>
@@ -561,10 +561,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="5">
         <v>45805</v>
@@ -572,10 +572,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="5">
         <v>45806</v>
@@ -583,10 +583,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5">
         <v>45807</v>
@@ -648,42 +648,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -712,145 +712,145 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -873,10 +873,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se prueba la ejecucion en un blucle while sin criterio de interrupcion
</commit_message>
<xml_diff>
--- a/facundo.xlsx
+++ b/facundo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\comedores_unr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14033E9-7160-4214-B092-57F11C89C1B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F814D0D-AD5B-4B44-A746-A3A5FA84BF7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{5C91FBF1-797B-4D74-8CDC-7038822E3838}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="menues" sheetId="1" r:id="rId1"/>
     <sheet name="comedores" sheetId="2" r:id="rId2"/>
     <sheet name="opciones_menu" sheetId="3" r:id="rId3"/>
-    <sheet name="fecha" sheetId="4" r:id="rId4"/>
+    <sheet name="fechas" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="agrotecnia">opciones_menu!$B$2:$B$13</definedName>
@@ -24,6 +24,7 @@
     <definedName name="centro">opciones_menu!$G$2:$G$13</definedName>
     <definedName name="comedores">comedores!$A$2:$A$8</definedName>
     <definedName name="fceia">opciones_menu!$D$2:$D$13</definedName>
+    <definedName name="fechas">fechas!$A$2:$A$6</definedName>
     <definedName name="salud">opciones_menu!$C$2:$C$13</definedName>
     <definedName name="siberia">opciones_menu!$A$2:$A$13</definedName>
     <definedName name="zaballa">opciones_menu!$E$2:$E$13</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="27">
   <si>
     <t>comedor</t>
   </si>
@@ -70,61 +71,64 @@
     <t>comedores</t>
   </si>
   <si>
-    <t>des</t>
+    <t>fecha</t>
   </si>
   <si>
-    <t>alm_llevar_14</t>
+    <t>desayuno (7:45 - 10.30)</t>
   </si>
   <si>
-    <t>alm_llevar_13</t>
+    <t>almuerzo (14 - 15)</t>
   </si>
   <si>
-    <t>alm_llevar_12</t>
+    <t>almuerzo (13 - 14)</t>
   </si>
   <si>
-    <t>alm_llevar_11</t>
+    <t>almuerzo (12 - 13)</t>
   </si>
   <si>
-    <t>alm_no_llevar_14</t>
+    <t>llevar almuerzo (14 - 15)</t>
   </si>
   <si>
-    <t>alm_no_llevar_13</t>
+    <t>llevar almuerzo (13 - 14)</t>
   </si>
   <si>
-    <t>alm_no_llevar_12</t>
+    <t>llevar almuerzo (12 - 13)</t>
   </si>
   <si>
-    <t>mer</t>
+    <t>merienda (16 - 19)</t>
   </si>
   <si>
-    <t>cen_llevar</t>
+    <t>llevar cena (19.30 - 21)</t>
   </si>
   <si>
-    <t>cen_no_llevar_20</t>
+    <t>cena (20 - 21)</t>
   </si>
   <si>
-    <t>cen_no_llevar_19.30</t>
+    <t>cena (19.30 - 20)</t>
   </si>
   <si>
-    <t>desde</t>
+    <t>merienda (16 - 18)</t>
   </si>
   <si>
-    <t>hasta</t>
+    <t>llevar almuerzo (11 - 12)</t>
   </si>
   <si>
-    <t>alm_llevar</t>
+    <t>llevar almuerzo (11 - 15)</t>
   </si>
   <si>
-    <t>cen_no_lleva</t>
+    <t>llevar cena (20 - 21)</t>
   </si>
   <si>
-    <t>fecha</t>
+    <t>fechas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-2C0A]dddd\,\ dd&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -175,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -184,8 +188,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -502,17 +509,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E57EADAA-D27F-4196-9F5D-6F9B5C2B1711}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C747"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -522,8 +529,8 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>26</v>
+      <c r="C1" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -531,10 +538,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="5">
-        <v>45803</v>
+        <v>11</v>
+      </c>
+      <c r="C2" s="6">
+        <v>45810</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -544,8 +551,8 @@
       <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="5">
-        <v>45803</v>
+      <c r="C3" s="6">
+        <v>45810</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -553,21 +560,21 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="5">
-        <v>45804</v>
+        <v>11</v>
+      </c>
+      <c r="C4" s="6">
+        <v>45811</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="5">
-        <v>45805</v>
+      <c r="C5" s="6">
+        <v>45811</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -575,57 +582,2288 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="5">
-        <v>45806</v>
+        <v>11</v>
+      </c>
+      <c r="C6" s="6">
+        <v>45812</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="6">
+        <v>45812</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="6">
+        <v>45813</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="5">
-        <v>45807</v>
-      </c>
+      <c r="C9" s="6">
+        <v>45813</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="6">
+        <v>45814</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="6">
+        <v>45814</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="6"/>
+    </row>
+    <row r="33" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="6"/>
+    </row>
+    <row r="35" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="6"/>
+    </row>
+    <row r="37" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="6"/>
+    </row>
+    <row r="40" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C42" s="6"/>
+    </row>
+    <row r="43" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C43" s="6"/>
+    </row>
+    <row r="44" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="6"/>
+    </row>
+    <row r="45" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C45" s="6"/>
+    </row>
+    <row r="46" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="6"/>
+    </row>
+    <row r="47" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="6"/>
+    </row>
+    <row r="48" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C48" s="6"/>
+    </row>
+    <row r="49" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C49" s="6"/>
+    </row>
+    <row r="50" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="6"/>
+    </row>
+    <row r="51" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C51" s="6"/>
+    </row>
+    <row r="52" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C52" s="6"/>
+    </row>
+    <row r="53" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C53" s="6"/>
+    </row>
+    <row r="54" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C54" s="6"/>
+    </row>
+    <row r="55" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C55" s="6"/>
+    </row>
+    <row r="56" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C56" s="6"/>
+    </row>
+    <row r="57" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C57" s="6"/>
+    </row>
+    <row r="58" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C58" s="6"/>
+    </row>
+    <row r="59" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C59" s="6"/>
+    </row>
+    <row r="60" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C60" s="6"/>
+    </row>
+    <row r="61" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C61" s="6"/>
+    </row>
+    <row r="62" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C62" s="6"/>
+    </row>
+    <row r="63" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C63" s="6"/>
+    </row>
+    <row r="64" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C64" s="6"/>
+    </row>
+    <row r="65" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C65" s="6"/>
+    </row>
+    <row r="66" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C66" s="6"/>
+    </row>
+    <row r="67" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C67" s="6"/>
+    </row>
+    <row r="68" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C68" s="6"/>
+    </row>
+    <row r="69" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C69" s="6"/>
+    </row>
+    <row r="70" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C70" s="6"/>
+    </row>
+    <row r="71" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C71" s="6"/>
+    </row>
+    <row r="72" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C72" s="6"/>
+    </row>
+    <row r="73" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C73" s="6"/>
+    </row>
+    <row r="74" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C74" s="6"/>
+    </row>
+    <row r="75" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C75" s="6"/>
+    </row>
+    <row r="76" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C76" s="6"/>
+    </row>
+    <row r="77" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C77" s="6"/>
+    </row>
+    <row r="78" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C78" s="6"/>
+    </row>
+    <row r="79" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C79" s="6"/>
+    </row>
+    <row r="80" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C80" s="6"/>
+    </row>
+    <row r="81" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C81" s="6"/>
+    </row>
+    <row r="82" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C82" s="6"/>
+    </row>
+    <row r="83" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C83" s="6"/>
+    </row>
+    <row r="84" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C84" s="6"/>
+    </row>
+    <row r="85" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C85" s="6"/>
+    </row>
+    <row r="86" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C86" s="6"/>
+    </row>
+    <row r="87" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C87" s="6"/>
+    </row>
+    <row r="88" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C88" s="6"/>
+    </row>
+    <row r="89" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C89" s="6"/>
+    </row>
+    <row r="90" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C90" s="6"/>
+    </row>
+    <row r="91" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C91" s="6"/>
+    </row>
+    <row r="92" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C92" s="6"/>
+    </row>
+    <row r="93" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C93" s="6"/>
+    </row>
+    <row r="94" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C94" s="6"/>
+    </row>
+    <row r="95" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C95" s="6"/>
+    </row>
+    <row r="96" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C96" s="6"/>
+    </row>
+    <row r="97" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C97" s="6"/>
+    </row>
+    <row r="98" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C98" s="6"/>
+    </row>
+    <row r="99" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C99" s="6"/>
+    </row>
+    <row r="100" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C100" s="6"/>
+    </row>
+    <row r="101" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C101" s="6"/>
+    </row>
+    <row r="102" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C102" s="6"/>
+    </row>
+    <row r="103" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C103" s="6"/>
+    </row>
+    <row r="104" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C104" s="6"/>
+    </row>
+    <row r="105" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C105" s="6"/>
+    </row>
+    <row r="106" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C106" s="6"/>
+    </row>
+    <row r="107" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C107" s="6"/>
+    </row>
+    <row r="108" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C108" s="6"/>
+    </row>
+    <row r="109" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C109" s="6"/>
+    </row>
+    <row r="110" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C110" s="6"/>
+    </row>
+    <row r="111" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C111" s="6"/>
+    </row>
+    <row r="112" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C112" s="6"/>
+    </row>
+    <row r="113" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C113" s="6"/>
+    </row>
+    <row r="114" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C114" s="6"/>
+    </row>
+    <row r="115" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C115" s="6"/>
+    </row>
+    <row r="116" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C116" s="6"/>
+    </row>
+    <row r="117" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C117" s="6"/>
+    </row>
+    <row r="118" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C118" s="6"/>
+    </row>
+    <row r="119" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C119" s="6"/>
+    </row>
+    <row r="120" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C120" s="6"/>
+    </row>
+    <row r="121" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C121" s="6"/>
+    </row>
+    <row r="122" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C122" s="6"/>
+    </row>
+    <row r="123" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C123" s="6"/>
+    </row>
+    <row r="124" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C124" s="6"/>
+    </row>
+    <row r="125" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C125" s="6"/>
+    </row>
+    <row r="126" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C126" s="6"/>
+    </row>
+    <row r="127" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C127" s="6"/>
+    </row>
+    <row r="128" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C128" s="6"/>
+    </row>
+    <row r="129" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C129" s="6"/>
+    </row>
+    <row r="130" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C130" s="6"/>
+    </row>
+    <row r="131" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C131" s="6"/>
+    </row>
+    <row r="132" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C132" s="6"/>
+    </row>
+    <row r="133" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C133" s="6"/>
+    </row>
+    <row r="134" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C134" s="6"/>
+    </row>
+    <row r="135" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C135" s="6"/>
+    </row>
+    <row r="136" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C136" s="6"/>
+    </row>
+    <row r="137" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C137" s="6"/>
+    </row>
+    <row r="138" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C138" s="6"/>
+    </row>
+    <row r="139" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C139" s="6"/>
+    </row>
+    <row r="140" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C140" s="6"/>
+    </row>
+    <row r="141" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C141" s="6"/>
+    </row>
+    <row r="142" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C142" s="6"/>
+    </row>
+    <row r="143" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C143" s="6"/>
+    </row>
+    <row r="144" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C144" s="6"/>
+    </row>
+    <row r="145" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C145" s="6"/>
+    </row>
+    <row r="146" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C146" s="6"/>
+    </row>
+    <row r="147" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C147" s="6"/>
+    </row>
+    <row r="148" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C148" s="6"/>
+    </row>
+    <row r="149" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C149" s="6"/>
+    </row>
+    <row r="150" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C150" s="6"/>
+    </row>
+    <row r="151" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C151" s="6"/>
+    </row>
+    <row r="152" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C152" s="6"/>
+    </row>
+    <row r="153" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C153" s="6"/>
+    </row>
+    <row r="154" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C154" s="6"/>
+    </row>
+    <row r="155" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C155" s="6"/>
+    </row>
+    <row r="156" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C156" s="6"/>
+    </row>
+    <row r="157" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C157" s="6"/>
+    </row>
+    <row r="158" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C158" s="6"/>
+    </row>
+    <row r="159" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C159" s="6"/>
+    </row>
+    <row r="160" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C160" s="6"/>
+    </row>
+    <row r="161" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C161" s="6"/>
+    </row>
+    <row r="162" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C162" s="6"/>
+    </row>
+    <row r="163" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C163" s="6"/>
+    </row>
+    <row r="164" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C164" s="6"/>
+    </row>
+    <row r="165" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C165" s="6"/>
+    </row>
+    <row r="166" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C166" s="6"/>
+    </row>
+    <row r="167" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C167" s="6"/>
+    </row>
+    <row r="168" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C168" s="6"/>
+    </row>
+    <row r="169" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C169" s="6"/>
+    </row>
+    <row r="170" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C170" s="6"/>
+    </row>
+    <row r="171" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C171" s="6"/>
+    </row>
+    <row r="172" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C172" s="6"/>
+    </row>
+    <row r="173" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C173" s="6"/>
+    </row>
+    <row r="174" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C174" s="6"/>
+    </row>
+    <row r="175" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C175" s="6"/>
+    </row>
+    <row r="176" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C176" s="6"/>
+    </row>
+    <row r="177" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C177" s="6"/>
+    </row>
+    <row r="178" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C178" s="6"/>
+    </row>
+    <row r="179" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C179" s="6"/>
+    </row>
+    <row r="180" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C180" s="6"/>
+    </row>
+    <row r="181" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C181" s="6"/>
+    </row>
+    <row r="182" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C182" s="6"/>
+    </row>
+    <row r="183" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C183" s="6"/>
+    </row>
+    <row r="184" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C184" s="6"/>
+    </row>
+    <row r="185" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C185" s="6"/>
+    </row>
+    <row r="186" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C186" s="6"/>
+    </row>
+    <row r="187" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C187" s="6"/>
+    </row>
+    <row r="188" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C188" s="6"/>
+    </row>
+    <row r="189" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C189" s="6"/>
+    </row>
+    <row r="190" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C190" s="6"/>
+    </row>
+    <row r="191" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C191" s="6"/>
+    </row>
+    <row r="192" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C192" s="6"/>
+    </row>
+    <row r="193" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C193" s="6"/>
+    </row>
+    <row r="194" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C194" s="6"/>
+    </row>
+    <row r="195" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C195" s="6"/>
+    </row>
+    <row r="196" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C196" s="6"/>
+    </row>
+    <row r="197" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C197" s="6"/>
+    </row>
+    <row r="198" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C198" s="6"/>
+    </row>
+    <row r="199" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C199" s="6"/>
+    </row>
+    <row r="200" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C200" s="6"/>
+    </row>
+    <row r="201" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C201" s="6"/>
+    </row>
+    <row r="202" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C202" s="6"/>
+    </row>
+    <row r="203" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C203" s="6"/>
+    </row>
+    <row r="204" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C204" s="6"/>
+    </row>
+    <row r="205" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C205" s="6"/>
+    </row>
+    <row r="206" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C206" s="6"/>
+    </row>
+    <row r="207" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C207" s="6"/>
+    </row>
+    <row r="208" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C208" s="6"/>
+    </row>
+    <row r="209" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C209" s="6"/>
+    </row>
+    <row r="210" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C210" s="6"/>
+    </row>
+    <row r="211" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C211" s="6"/>
+    </row>
+    <row r="212" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C212" s="6"/>
+    </row>
+    <row r="213" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C213" s="6"/>
+    </row>
+    <row r="214" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C214" s="6"/>
+    </row>
+    <row r="215" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C215" s="6"/>
+    </row>
+    <row r="216" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C216" s="6"/>
+    </row>
+    <row r="217" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C217" s="6"/>
+    </row>
+    <row r="218" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C218" s="6"/>
+    </row>
+    <row r="219" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C219" s="6"/>
+    </row>
+    <row r="220" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C220" s="6"/>
+    </row>
+    <row r="221" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C221" s="6"/>
+    </row>
+    <row r="222" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C222" s="6"/>
+    </row>
+    <row r="223" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C223" s="6"/>
+    </row>
+    <row r="224" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C224" s="6"/>
+    </row>
+    <row r="225" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C225" s="6"/>
+    </row>
+    <row r="226" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C226" s="6"/>
+    </row>
+    <row r="227" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C227" s="6"/>
+    </row>
+    <row r="228" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C228" s="6"/>
+    </row>
+    <row r="229" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C229" s="6"/>
+    </row>
+    <row r="230" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C230" s="6"/>
+    </row>
+    <row r="231" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C231" s="6"/>
+    </row>
+    <row r="232" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C232" s="6"/>
+    </row>
+    <row r="233" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C233" s="6"/>
+    </row>
+    <row r="234" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C234" s="6"/>
+    </row>
+    <row r="235" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C235" s="6"/>
+    </row>
+    <row r="236" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C236" s="6"/>
+    </row>
+    <row r="237" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C237" s="6"/>
+    </row>
+    <row r="238" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C238" s="6"/>
+    </row>
+    <row r="239" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C239" s="6"/>
+    </row>
+    <row r="240" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C240" s="6"/>
+    </row>
+    <row r="241" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C241" s="6"/>
+    </row>
+    <row r="242" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C242" s="6"/>
+    </row>
+    <row r="243" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C243" s="6"/>
+    </row>
+    <row r="244" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C244" s="6"/>
+    </row>
+    <row r="245" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C245" s="6"/>
+    </row>
+    <row r="246" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C246" s="6"/>
+    </row>
+    <row r="247" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C247" s="6"/>
+    </row>
+    <row r="248" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C248" s="6"/>
+    </row>
+    <row r="249" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C249" s="6"/>
+    </row>
+    <row r="250" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C250" s="6"/>
+    </row>
+    <row r="251" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C251" s="6"/>
+    </row>
+    <row r="252" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C252" s="6"/>
+    </row>
+    <row r="253" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C253" s="6"/>
+    </row>
+    <row r="254" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C254" s="6"/>
+    </row>
+    <row r="255" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C255" s="6"/>
+    </row>
+    <row r="256" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C256" s="6"/>
+    </row>
+    <row r="257" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C257" s="6"/>
+    </row>
+    <row r="258" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C258" s="6"/>
+    </row>
+    <row r="259" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C259" s="6"/>
+    </row>
+    <row r="260" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C260" s="6"/>
+    </row>
+    <row r="261" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C261" s="6"/>
+    </row>
+    <row r="262" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C262" s="6"/>
+    </row>
+    <row r="263" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C263" s="6"/>
+    </row>
+    <row r="264" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C264" s="6"/>
+    </row>
+    <row r="265" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C265" s="6"/>
+    </row>
+    <row r="266" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C266" s="6"/>
+    </row>
+    <row r="267" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C267" s="6"/>
+    </row>
+    <row r="268" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C268" s="6"/>
+    </row>
+    <row r="269" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C269" s="6"/>
+    </row>
+    <row r="270" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C270" s="6"/>
+    </row>
+    <row r="271" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C271" s="6"/>
+    </row>
+    <row r="272" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C272" s="6"/>
+    </row>
+    <row r="273" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C273" s="6"/>
+    </row>
+    <row r="274" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C274" s="6"/>
+    </row>
+    <row r="275" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C275" s="6"/>
+    </row>
+    <row r="276" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C276" s="6"/>
+    </row>
+    <row r="277" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C277" s="6"/>
+    </row>
+    <row r="278" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C278" s="6"/>
+    </row>
+    <row r="279" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C279" s="6"/>
+    </row>
+    <row r="280" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C280" s="6"/>
+    </row>
+    <row r="281" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C281" s="6"/>
+    </row>
+    <row r="282" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C282" s="6"/>
+    </row>
+    <row r="283" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C283" s="6"/>
+    </row>
+    <row r="284" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C284" s="6"/>
+    </row>
+    <row r="285" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C285" s="6"/>
+    </row>
+    <row r="286" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C286" s="6"/>
+    </row>
+    <row r="287" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C287" s="6"/>
+    </row>
+    <row r="288" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C288" s="6"/>
+    </row>
+    <row r="289" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C289" s="6"/>
+    </row>
+    <row r="290" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C290" s="6"/>
+    </row>
+    <row r="291" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C291" s="6"/>
+    </row>
+    <row r="292" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C292" s="6"/>
+    </row>
+    <row r="293" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C293" s="6"/>
+    </row>
+    <row r="294" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C294" s="6"/>
+    </row>
+    <row r="295" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C295" s="6"/>
+    </row>
+    <row r="296" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C296" s="6"/>
+    </row>
+    <row r="297" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C297" s="6"/>
+    </row>
+    <row r="298" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C298" s="6"/>
+    </row>
+    <row r="299" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C299" s="6"/>
+    </row>
+    <row r="300" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C300" s="6"/>
+    </row>
+    <row r="301" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C301" s="6"/>
+    </row>
+    <row r="302" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C302" s="6"/>
+    </row>
+    <row r="303" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C303" s="6"/>
+    </row>
+    <row r="304" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C304" s="6"/>
+    </row>
+    <row r="305" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C305" s="6"/>
+    </row>
+    <row r="306" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C306" s="6"/>
+    </row>
+    <row r="307" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C307" s="6"/>
+    </row>
+    <row r="308" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C308" s="6"/>
+    </row>
+    <row r="309" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C309" s="6"/>
+    </row>
+    <row r="310" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C310" s="6"/>
+    </row>
+    <row r="311" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C311" s="6"/>
+    </row>
+    <row r="312" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C312" s="6"/>
+    </row>
+    <row r="313" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C313" s="6"/>
+    </row>
+    <row r="314" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C314" s="6"/>
+    </row>
+    <row r="315" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C315" s="6"/>
+    </row>
+    <row r="316" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C316" s="6"/>
+    </row>
+    <row r="317" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C317" s="6"/>
+    </row>
+    <row r="318" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C318" s="6"/>
+    </row>
+    <row r="319" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C319" s="6"/>
+    </row>
+    <row r="320" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C320" s="6"/>
+    </row>
+    <row r="321" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C321" s="6"/>
+    </row>
+    <row r="322" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C322" s="6"/>
+    </row>
+    <row r="323" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C323" s="6"/>
+    </row>
+    <row r="324" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C324" s="6"/>
+    </row>
+    <row r="325" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C325" s="6"/>
+    </row>
+    <row r="326" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C326" s="6"/>
+    </row>
+    <row r="327" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C327" s="6"/>
+    </row>
+    <row r="328" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C328" s="6"/>
+    </row>
+    <row r="329" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C329" s="6"/>
+    </row>
+    <row r="330" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C330" s="6"/>
+    </row>
+    <row r="331" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C331" s="6"/>
+    </row>
+    <row r="332" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C332" s="6"/>
+    </row>
+    <row r="333" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C333" s="6"/>
+    </row>
+    <row r="334" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C334" s="6"/>
+    </row>
+    <row r="335" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C335" s="6"/>
+    </row>
+    <row r="336" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C336" s="6"/>
+    </row>
+    <row r="337" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C337" s="6"/>
+    </row>
+    <row r="338" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C338" s="6"/>
+    </row>
+    <row r="339" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C339" s="6"/>
+    </row>
+    <row r="340" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C340" s="6"/>
+    </row>
+    <row r="341" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C341" s="6"/>
+    </row>
+    <row r="342" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C342" s="6"/>
+    </row>
+    <row r="343" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C343" s="6"/>
+    </row>
+    <row r="344" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C344" s="6"/>
+    </row>
+    <row r="345" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C345" s="6"/>
+    </row>
+    <row r="346" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C346" s="6"/>
+    </row>
+    <row r="347" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C347" s="6"/>
+    </row>
+    <row r="348" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C348" s="6"/>
+    </row>
+    <row r="349" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C349" s="6"/>
+    </row>
+    <row r="350" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C350" s="6"/>
+    </row>
+    <row r="351" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C351" s="6"/>
+    </row>
+    <row r="352" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C352" s="6"/>
+    </row>
+    <row r="353" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C353" s="6"/>
+    </row>
+    <row r="354" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C354" s="6"/>
+    </row>
+    <row r="355" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C355" s="6"/>
+    </row>
+    <row r="356" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C356" s="6"/>
+    </row>
+    <row r="357" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C357" s="6"/>
+    </row>
+    <row r="358" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C358" s="6"/>
+    </row>
+    <row r="359" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C359" s="6"/>
+    </row>
+    <row r="360" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C360" s="6"/>
+    </row>
+    <row r="361" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C361" s="6"/>
+    </row>
+    <row r="362" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C362" s="6"/>
+    </row>
+    <row r="363" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C363" s="6"/>
+    </row>
+    <row r="364" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C364" s="6"/>
+    </row>
+    <row r="365" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C365" s="6"/>
+    </row>
+    <row r="366" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C366" s="6"/>
+    </row>
+    <row r="367" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C367" s="6"/>
+    </row>
+    <row r="368" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C368" s="6"/>
+    </row>
+    <row r="369" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C369" s="6"/>
+    </row>
+    <row r="370" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C370" s="6"/>
+    </row>
+    <row r="371" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C371" s="6"/>
+    </row>
+    <row r="372" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C372" s="6"/>
+    </row>
+    <row r="373" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C373" s="6"/>
+    </row>
+    <row r="374" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C374" s="6"/>
+    </row>
+    <row r="375" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C375" s="6"/>
+    </row>
+    <row r="376" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C376" s="6"/>
+    </row>
+    <row r="377" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C377" s="6"/>
+    </row>
+    <row r="378" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C378" s="6"/>
+    </row>
+    <row r="379" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C379" s="6"/>
+    </row>
+    <row r="380" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C380" s="6"/>
+    </row>
+    <row r="381" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C381" s="6"/>
+    </row>
+    <row r="382" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C382" s="6"/>
+    </row>
+    <row r="383" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C383" s="6"/>
+    </row>
+    <row r="384" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C384" s="6"/>
+    </row>
+    <row r="385" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C385" s="6"/>
+    </row>
+    <row r="386" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C386" s="6"/>
+    </row>
+    <row r="387" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C387" s="6"/>
+    </row>
+    <row r="388" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C388" s="6"/>
+    </row>
+    <row r="389" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C389" s="6"/>
+    </row>
+    <row r="390" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C390" s="6"/>
+    </row>
+    <row r="391" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C391" s="6"/>
+    </row>
+    <row r="392" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C392" s="6"/>
+    </row>
+    <row r="393" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C393" s="6"/>
+    </row>
+    <row r="394" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C394" s="6"/>
+    </row>
+    <row r="395" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C395" s="6"/>
+    </row>
+    <row r="396" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C396" s="6"/>
+    </row>
+    <row r="397" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C397" s="6"/>
+    </row>
+    <row r="398" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C398" s="6"/>
+    </row>
+    <row r="399" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C399" s="6"/>
+    </row>
+    <row r="400" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C400" s="6"/>
+    </row>
+    <row r="401" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C401" s="6"/>
+    </row>
+    <row r="402" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C402" s="6"/>
+    </row>
+    <row r="403" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C403" s="6"/>
+    </row>
+    <row r="404" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C404" s="6"/>
+    </row>
+    <row r="405" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C405" s="6"/>
+    </row>
+    <row r="406" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C406" s="6"/>
+    </row>
+    <row r="407" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C407" s="6"/>
+    </row>
+    <row r="408" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C408" s="6"/>
+    </row>
+    <row r="409" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C409" s="6"/>
+    </row>
+    <row r="410" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C410" s="6"/>
+    </row>
+    <row r="411" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C411" s="6"/>
+    </row>
+    <row r="412" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C412" s="6"/>
+    </row>
+    <row r="413" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C413" s="6"/>
+    </row>
+    <row r="414" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C414" s="6"/>
+    </row>
+    <row r="415" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C415" s="6"/>
+    </row>
+    <row r="416" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C416" s="6"/>
+    </row>
+    <row r="417" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C417" s="6"/>
+    </row>
+    <row r="418" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C418" s="6"/>
+    </row>
+    <row r="419" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C419" s="6"/>
+    </row>
+    <row r="420" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C420" s="6"/>
+    </row>
+    <row r="421" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C421" s="6"/>
+    </row>
+    <row r="422" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C422" s="6"/>
+    </row>
+    <row r="423" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C423" s="6"/>
+    </row>
+    <row r="424" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C424" s="6"/>
+    </row>
+    <row r="425" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C425" s="6"/>
+    </row>
+    <row r="426" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C426" s="6"/>
+    </row>
+    <row r="427" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C427" s="6"/>
+    </row>
+    <row r="428" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C428" s="6"/>
+    </row>
+    <row r="429" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C429" s="6"/>
+    </row>
+    <row r="430" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C430" s="6"/>
+    </row>
+    <row r="431" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C431" s="6"/>
+    </row>
+    <row r="432" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C432" s="6"/>
+    </row>
+    <row r="433" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C433" s="6"/>
+    </row>
+    <row r="434" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C434" s="6"/>
+    </row>
+    <row r="435" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C435" s="6"/>
+    </row>
+    <row r="436" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C436" s="6"/>
+    </row>
+    <row r="437" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C437" s="6"/>
+    </row>
+    <row r="438" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C438" s="6"/>
+    </row>
+    <row r="439" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C439" s="6"/>
+    </row>
+    <row r="440" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C440" s="6"/>
+    </row>
+    <row r="441" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C441" s="6"/>
+    </row>
+    <row r="442" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C442" s="6"/>
+    </row>
+    <row r="443" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C443" s="6"/>
+    </row>
+    <row r="444" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C444" s="6"/>
+    </row>
+    <row r="445" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C445" s="6"/>
+    </row>
+    <row r="446" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C446" s="6"/>
+    </row>
+    <row r="447" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C447" s="6"/>
+    </row>
+    <row r="448" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C448" s="6"/>
+    </row>
+    <row r="449" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C449" s="6"/>
+    </row>
+    <row r="450" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C450" s="6"/>
+    </row>
+    <row r="451" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C451" s="6"/>
+    </row>
+    <row r="452" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C452" s="6"/>
+    </row>
+    <row r="453" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C453" s="6"/>
+    </row>
+    <row r="454" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C454" s="6"/>
+    </row>
+    <row r="455" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C455" s="6"/>
+    </row>
+    <row r="456" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C456" s="6"/>
+    </row>
+    <row r="457" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C457" s="6"/>
+    </row>
+    <row r="458" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C458" s="6"/>
+    </row>
+    <row r="459" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C459" s="6"/>
+    </row>
+    <row r="460" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C460" s="6"/>
+    </row>
+    <row r="461" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C461" s="6"/>
+    </row>
+    <row r="462" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C462" s="6"/>
+    </row>
+    <row r="463" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C463" s="6"/>
+    </row>
+    <row r="464" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C464" s="6"/>
+    </row>
+    <row r="465" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C465" s="6"/>
+    </row>
+    <row r="466" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C466" s="6"/>
+    </row>
+    <row r="467" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C467" s="6"/>
+    </row>
+    <row r="468" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C468" s="6"/>
+    </row>
+    <row r="469" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C469" s="6"/>
+    </row>
+    <row r="470" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C470" s="6"/>
+    </row>
+    <row r="471" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C471" s="6"/>
+    </row>
+    <row r="472" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C472" s="6"/>
+    </row>
+    <row r="473" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C473" s="6"/>
+    </row>
+    <row r="474" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C474" s="6"/>
+    </row>
+    <row r="475" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C475" s="6"/>
+    </row>
+    <row r="476" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C476" s="6"/>
+    </row>
+    <row r="477" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C477" s="6"/>
+    </row>
+    <row r="478" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C478" s="6"/>
+    </row>
+    <row r="479" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C479" s="6"/>
+    </row>
+    <row r="480" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C480" s="6"/>
+    </row>
+    <row r="481" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C481" s="6"/>
+    </row>
+    <row r="482" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C482" s="6"/>
+    </row>
+    <row r="483" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C483" s="6"/>
+    </row>
+    <row r="484" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C484" s="6"/>
+    </row>
+    <row r="485" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C485" s="6"/>
+    </row>
+    <row r="486" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C486" s="6"/>
+    </row>
+    <row r="487" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C487" s="6"/>
+    </row>
+    <row r="488" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C488" s="6"/>
+    </row>
+    <row r="489" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C489" s="6"/>
+    </row>
+    <row r="490" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C490" s="6"/>
+    </row>
+    <row r="491" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C491" s="6"/>
+    </row>
+    <row r="492" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C492" s="6"/>
+    </row>
+    <row r="493" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C493" s="6"/>
+    </row>
+    <row r="494" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C494" s="6"/>
+    </row>
+    <row r="495" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C495" s="6"/>
+    </row>
+    <row r="496" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C496" s="6"/>
+    </row>
+    <row r="497" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C497" s="6"/>
+    </row>
+    <row r="498" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C498" s="6"/>
+    </row>
+    <row r="499" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C499" s="6"/>
+    </row>
+    <row r="500" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C500" s="6"/>
+    </row>
+    <row r="501" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C501" s="6"/>
+    </row>
+    <row r="502" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C502" s="6"/>
+    </row>
+    <row r="503" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C503" s="6"/>
+    </row>
+    <row r="504" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C504" s="6"/>
+    </row>
+    <row r="505" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C505" s="6"/>
+    </row>
+    <row r="506" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C506" s="6"/>
+    </row>
+    <row r="507" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C507" s="6"/>
+    </row>
+    <row r="508" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C508" s="6"/>
+    </row>
+    <row r="509" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C509" s="6"/>
+    </row>
+    <row r="510" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C510" s="6"/>
+    </row>
+    <row r="511" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C511" s="6"/>
+    </row>
+    <row r="512" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C512" s="6"/>
+    </row>
+    <row r="513" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C513" s="6"/>
+    </row>
+    <row r="514" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C514" s="6"/>
+    </row>
+    <row r="515" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C515" s="6"/>
+    </row>
+    <row r="516" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C516" s="6"/>
+    </row>
+    <row r="517" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C517" s="6"/>
+    </row>
+    <row r="518" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C518" s="6"/>
+    </row>
+    <row r="519" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C519" s="6"/>
+    </row>
+    <row r="520" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C520" s="6"/>
+    </row>
+    <row r="521" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C521" s="6"/>
+    </row>
+    <row r="522" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C522" s="6"/>
+    </row>
+    <row r="523" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C523" s="6"/>
+    </row>
+    <row r="524" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C524" s="6"/>
+    </row>
+    <row r="525" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C525" s="6"/>
+    </row>
+    <row r="526" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C526" s="6"/>
+    </row>
+    <row r="527" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C527" s="6"/>
+    </row>
+    <row r="528" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C528" s="6"/>
+    </row>
+    <row r="529" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C529" s="6"/>
+    </row>
+    <row r="530" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C530" s="6"/>
+    </row>
+    <row r="531" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C531" s="6"/>
+    </row>
+    <row r="532" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C532" s="6"/>
+    </row>
+    <row r="533" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C533" s="6"/>
+    </row>
+    <row r="534" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C534" s="6"/>
+    </row>
+    <row r="535" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C535" s="6"/>
+    </row>
+    <row r="536" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C536" s="6"/>
+    </row>
+    <row r="537" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C537" s="6"/>
+    </row>
+    <row r="538" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C538" s="6"/>
+    </row>
+    <row r="539" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C539" s="6"/>
+    </row>
+    <row r="540" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C540" s="6"/>
+    </row>
+    <row r="541" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C541" s="6"/>
+    </row>
+    <row r="542" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C542" s="6"/>
+    </row>
+    <row r="543" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C543" s="6"/>
+    </row>
+    <row r="544" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C544" s="6"/>
+    </row>
+    <row r="545" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C545" s="6"/>
+    </row>
+    <row r="546" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C546" s="6"/>
+    </row>
+    <row r="547" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C547" s="6"/>
+    </row>
+    <row r="548" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C548" s="6"/>
+    </row>
+    <row r="549" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C549" s="6"/>
+    </row>
+    <row r="550" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C550" s="6"/>
+    </row>
+    <row r="551" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C551" s="6"/>
+    </row>
+    <row r="552" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C552" s="6"/>
+    </row>
+    <row r="553" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C553" s="6"/>
+    </row>
+    <row r="554" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C554" s="6"/>
+    </row>
+    <row r="555" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C555" s="6"/>
+    </row>
+    <row r="556" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C556" s="6"/>
+    </row>
+    <row r="557" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C557" s="6"/>
+    </row>
+    <row r="558" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C558" s="6"/>
+    </row>
+    <row r="559" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C559" s="6"/>
+    </row>
+    <row r="560" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C560" s="6"/>
+    </row>
+    <row r="561" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C561" s="6"/>
+    </row>
+    <row r="562" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C562" s="6"/>
+    </row>
+    <row r="563" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C563" s="6"/>
+    </row>
+    <row r="564" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C564" s="6"/>
+    </row>
+    <row r="565" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C565" s="6"/>
+    </row>
+    <row r="566" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C566" s="6"/>
+    </row>
+    <row r="567" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C567" s="6"/>
+    </row>
+    <row r="568" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C568" s="6"/>
+    </row>
+    <row r="569" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C569" s="6"/>
+    </row>
+    <row r="570" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C570" s="6"/>
+    </row>
+    <row r="571" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C571" s="6"/>
+    </row>
+    <row r="572" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C572" s="6"/>
+    </row>
+    <row r="573" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C573" s="6"/>
+    </row>
+    <row r="574" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C574" s="6"/>
+    </row>
+    <row r="575" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C575" s="6"/>
+    </row>
+    <row r="576" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C576" s="6"/>
+    </row>
+    <row r="577" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C577" s="6"/>
+    </row>
+    <row r="578" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C578" s="6"/>
+    </row>
+    <row r="579" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C579" s="6"/>
+    </row>
+    <row r="580" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C580" s="6"/>
+    </row>
+    <row r="581" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C581" s="6"/>
+    </row>
+    <row r="582" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C582" s="6"/>
+    </row>
+    <row r="583" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C583" s="6"/>
+    </row>
+    <row r="584" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C584" s="6"/>
+    </row>
+    <row r="585" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C585" s="6"/>
+    </row>
+    <row r="586" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C586" s="6"/>
+    </row>
+    <row r="587" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C587" s="6"/>
+    </row>
+    <row r="588" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C588" s="6"/>
+    </row>
+    <row r="589" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C589" s="6"/>
+    </row>
+    <row r="590" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C590" s="6"/>
+    </row>
+    <row r="591" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C591" s="6"/>
+    </row>
+    <row r="592" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C592" s="6"/>
+    </row>
+    <row r="593" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C593" s="6"/>
+    </row>
+    <row r="594" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C594" s="6"/>
+    </row>
+    <row r="595" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C595" s="6"/>
+    </row>
+    <row r="596" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C596" s="6"/>
+    </row>
+    <row r="597" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C597" s="6"/>
+    </row>
+    <row r="598" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C598" s="6"/>
+    </row>
+    <row r="599" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C599" s="6"/>
+    </row>
+    <row r="600" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C600" s="6"/>
+    </row>
+    <row r="601" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C601" s="6"/>
+    </row>
+    <row r="602" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C602" s="6"/>
+    </row>
+    <row r="603" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C603" s="6"/>
+    </row>
+    <row r="604" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C604" s="6"/>
+    </row>
+    <row r="605" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C605" s="6"/>
+    </row>
+    <row r="606" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C606" s="6"/>
+    </row>
+    <row r="607" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C607" s="6"/>
+    </row>
+    <row r="608" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C608" s="6"/>
+    </row>
+    <row r="609" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C609" s="6"/>
+    </row>
+    <row r="610" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C610" s="6"/>
+    </row>
+    <row r="611" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C611" s="6"/>
+    </row>
+    <row r="612" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C612" s="6"/>
+    </row>
+    <row r="613" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C613" s="6"/>
+    </row>
+    <row r="614" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C614" s="6"/>
+    </row>
+    <row r="615" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C615" s="6"/>
+    </row>
+    <row r="616" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C616" s="6"/>
+    </row>
+    <row r="617" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C617" s="6"/>
+    </row>
+    <row r="618" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C618" s="6"/>
+    </row>
+    <row r="619" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C619" s="6"/>
+    </row>
+    <row r="620" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C620" s="6"/>
+    </row>
+    <row r="621" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C621" s="6"/>
+    </row>
+    <row r="622" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C622" s="6"/>
+    </row>
+    <row r="623" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C623" s="6"/>
+    </row>
+    <row r="624" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C624" s="6"/>
+    </row>
+    <row r="625" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C625" s="6"/>
+    </row>
+    <row r="626" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C626" s="6"/>
+    </row>
+    <row r="627" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C627" s="6"/>
+    </row>
+    <row r="628" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C628" s="6"/>
+    </row>
+    <row r="629" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C629" s="6"/>
+    </row>
+    <row r="630" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C630" s="6"/>
+    </row>
+    <row r="631" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C631" s="6"/>
+    </row>
+    <row r="632" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C632" s="6"/>
+    </row>
+    <row r="633" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C633" s="6"/>
+    </row>
+    <row r="634" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C634" s="6"/>
+    </row>
+    <row r="635" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C635" s="6"/>
+    </row>
+    <row r="636" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C636" s="6"/>
+    </row>
+    <row r="637" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C637" s="6"/>
+    </row>
+    <row r="638" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C638" s="6"/>
+    </row>
+    <row r="639" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C639" s="6"/>
+    </row>
+    <row r="640" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C640" s="6"/>
+    </row>
+    <row r="641" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C641" s="6"/>
+    </row>
+    <row r="642" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C642" s="6"/>
+    </row>
+    <row r="643" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C643" s="6"/>
+    </row>
+    <row r="644" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C644" s="6"/>
+    </row>
+    <row r="645" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C645" s="6"/>
+    </row>
+    <row r="646" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C646" s="6"/>
+    </row>
+    <row r="647" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C647" s="6"/>
+    </row>
+    <row r="648" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C648" s="6"/>
+    </row>
+    <row r="649" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C649" s="6"/>
+    </row>
+    <row r="650" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C650" s="6"/>
+    </row>
+    <row r="651" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C651" s="6"/>
+    </row>
+    <row r="652" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C652" s="6"/>
+    </row>
+    <row r="653" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C653" s="6"/>
+    </row>
+    <row r="654" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C654" s="6"/>
+    </row>
+    <row r="655" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C655" s="6"/>
+    </row>
+    <row r="656" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C656" s="6"/>
+    </row>
+    <row r="657" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C657" s="6"/>
+    </row>
+    <row r="658" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C658" s="6"/>
+    </row>
+    <row r="659" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C659" s="6"/>
+    </row>
+    <row r="660" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C660" s="6"/>
+    </row>
+    <row r="661" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C661" s="6"/>
+    </row>
+    <row r="662" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C662" s="6"/>
+    </row>
+    <row r="663" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C663" s="6"/>
+    </row>
+    <row r="664" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C664" s="6"/>
+    </row>
+    <row r="665" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C665" s="6"/>
+    </row>
+    <row r="666" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C666" s="6"/>
+    </row>
+    <row r="667" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C667" s="6"/>
+    </row>
+    <row r="668" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C668" s="6"/>
+    </row>
+    <row r="669" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C669" s="6"/>
+    </row>
+    <row r="670" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C670" s="6"/>
+    </row>
+    <row r="671" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C671" s="6"/>
+    </row>
+    <row r="672" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C672" s="6"/>
+    </row>
+    <row r="673" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C673" s="6"/>
+    </row>
+    <row r="674" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C674" s="6"/>
+    </row>
+    <row r="675" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C675" s="6"/>
+    </row>
+    <row r="676" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C676" s="6"/>
+    </row>
+    <row r="677" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C677" s="6"/>
+    </row>
+    <row r="678" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C678" s="6"/>
+    </row>
+    <row r="679" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C679" s="6"/>
+    </row>
+    <row r="680" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C680" s="6"/>
+    </row>
+    <row r="681" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C681" s="6"/>
+    </row>
+    <row r="682" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C682" s="6"/>
+    </row>
+    <row r="683" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C683" s="6"/>
+    </row>
+    <row r="684" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C684" s="6"/>
+    </row>
+    <row r="685" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C685" s="6"/>
+    </row>
+    <row r="686" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C686" s="6"/>
+    </row>
+    <row r="687" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C687" s="6"/>
+    </row>
+    <row r="688" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C688" s="6"/>
+    </row>
+    <row r="689" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C689" s="6"/>
+    </row>
+    <row r="690" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C690" s="6"/>
+    </row>
+    <row r="691" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C691" s="6"/>
+    </row>
+    <row r="692" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C692" s="6"/>
+    </row>
+    <row r="693" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C693" s="6"/>
+    </row>
+    <row r="694" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C694" s="6"/>
+    </row>
+    <row r="695" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C695" s="6"/>
+    </row>
+    <row r="696" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C696" s="6"/>
+    </row>
+    <row r="697" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C697" s="6"/>
+    </row>
+    <row r="698" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C698" s="6"/>
+    </row>
+    <row r="699" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C699" s="6"/>
+    </row>
+    <row r="700" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C700" s="6"/>
+    </row>
+    <row r="701" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C701" s="6"/>
+    </row>
+    <row r="702" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C702" s="6"/>
+    </row>
+    <row r="703" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C703" s="6"/>
+    </row>
+    <row r="704" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C704" s="6"/>
+    </row>
+    <row r="705" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C705" s="6"/>
+    </row>
+    <row r="706" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C706" s="6"/>
+    </row>
+    <row r="707" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C707" s="6"/>
+    </row>
+    <row r="708" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C708" s="6"/>
+    </row>
+    <row r="709" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C709" s="6"/>
+    </row>
+    <row r="710" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C710" s="6"/>
+    </row>
+    <row r="711" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C711" s="6"/>
+    </row>
+    <row r="712" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C712" s="6"/>
+    </row>
+    <row r="713" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C713" s="6"/>
+    </row>
+    <row r="714" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C714" s="6"/>
+    </row>
+    <row r="715" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C715" s="6"/>
+    </row>
+    <row r="716" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C716" s="6"/>
+    </row>
+    <row r="717" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C717" s="6"/>
+    </row>
+    <row r="718" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C718" s="6"/>
+    </row>
+    <row r="719" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C719" s="6"/>
+    </row>
+    <row r="720" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C720" s="6"/>
+    </row>
+    <row r="721" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C721" s="6"/>
+    </row>
+    <row r="722" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C722" s="6"/>
+    </row>
+    <row r="723" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C723" s="6"/>
+    </row>
+    <row r="724" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C724" s="6"/>
+    </row>
+    <row r="725" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C725" s="6"/>
+    </row>
+    <row r="726" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C726" s="6"/>
+    </row>
+    <row r="727" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C727" s="6"/>
+    </row>
+    <row r="728" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C728" s="6"/>
+    </row>
+    <row r="729" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C729" s="6"/>
+    </row>
+    <row r="730" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C730" s="6"/>
+    </row>
+    <row r="731" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C731" s="6"/>
+    </row>
+    <row r="732" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C732" s="6"/>
+    </row>
+    <row r="733" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C733" s="6"/>
+    </row>
+    <row r="734" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C734" s="6"/>
+    </row>
+    <row r="735" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C735" s="6"/>
+    </row>
+    <row r="736" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C736" s="6"/>
+    </row>
+    <row r="737" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C737" s="6"/>
+    </row>
+    <row r="738" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C738" s="6"/>
+    </row>
+    <row r="739" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C739" s="6"/>
+    </row>
+    <row r="740" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C740" s="6"/>
+    </row>
+    <row r="741" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C741" s="6"/>
+    </row>
+    <row r="742" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C742" s="6"/>
+    </row>
+    <row r="743" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C743" s="6"/>
+    </row>
+    <row r="744" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C744" s="6"/>
+    </row>
+    <row r="745" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C745" s="6"/>
+    </row>
+    <row r="746" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C746" s="6"/>
+    </row>
+    <row r="747" spans="3:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C747" s="6"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B858:B1048576" xr:uid="{531AE5A0-EC89-48F8-A3E5-33FE2ABF0ED1}">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{10A41909-0E0A-4314-8207-4DA0B7C8508D}">
       <formula1>comedores</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B865:B1048576" xr:uid="{531AE5A0-EC89-48F8-A3E5-33FE2ABF0ED1}">
-      <formula1>INDIRECT($A$2)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B857" xr:uid="{16E48105-2273-4AEA-A8CC-0B45FAF705D5}">
+      <formula1>INDIRECT(A2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B864" xr:uid="{16E48105-2273-4AEA-A8CC-0B45FAF705D5}">
-      <formula1>INDIRECT(A2)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C747" xr:uid="{E0DE0EAF-91D8-4659-A19F-B68973C47013}">
+      <formula1>fechas</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E0DE0EAF-91D8-4659-A19F-B68973C47013}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F3F5093F-5F34-4818-8517-C09E64BC83B2}">
           <x14:formula1>
-            <xm:f>fecha!A2</xm:f>
+            <xm:f>fechas!A747</xm:f>
           </x14:formula1>
           <x14:formula2>
-            <xm:f>fecha!B2</xm:f>
+            <xm:f>fechas!#REF!</xm:f>
           </x14:formula2>
-          <xm:sqref>C2:C3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F3F5093F-5F34-4818-8517-C09E64BC83B2}">
-          <x14:formula1>
-            <xm:f>fecha!A3</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>fecha!B3</xm:f>
-          </x14:formula2>
-          <xm:sqref>C4:C1048576</xm:sqref>
+          <xm:sqref>C748:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -638,7 +2876,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,18 +2934,17 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -735,97 +2972,124 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
         <v>24</v>
       </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
+      <c r="G4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
+      <c r="G5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
+      <c r="G6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
       </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" t="s">
+      <c r="G10" t="s">
         <v>18</v>
       </c>
     </row>
@@ -836,6 +3100,9 @@
       <c r="C11" t="s">
         <v>19</v>
       </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -844,12 +3111,18 @@
       <c r="C12" t="s">
         <v>20</v>
       </c>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
       <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" t="s">
         <v>21</v>
       </c>
     </row>
@@ -860,34 +3133,55 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34240258-DC70-4365-94CE-11F231A066AD}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>45803</v>
-      </c>
-      <c r="B2" s="4">
-        <v>45807</v>
-      </c>
+        <v>45810</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>45811</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>45812</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>45813</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>45814</v>
+      </c>
+      <c r="C6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>